<commit_message>
Detecting errors on load_from_json
</commit_message>
<xml_diff>
--- a/bdd_project.xlsx
+++ b/bdd_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfc/Documents/OpenSimula/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42276EC2-310A-0544-BAC7-F67D6BCF6728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF77AD6-0521-6040-9FA6-D14638CF082D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11000" yWindow="2700" windowWidth="28040" windowHeight="17440" xr2:uid="{A05B1B0C-29E4-C040-A1DF-87EBD9366E7D}"/>
+    <workbookView xWindow="11000" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{A05B1B0C-29E4-C040-A1DF-87EBD9366E7D}"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -47,70 +47,70 @@
     <t>value</t>
   </si>
   <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Base de Datos</t>
+  </si>
+  <si>
+    <t>zonaB4</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>meteo/zonaB4.met</t>
+  </si>
+  <si>
+    <t>Mortero cemento</t>
+  </si>
+  <si>
+    <t>Ladrillo hueco</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>specific_heat</t>
+  </si>
+  <si>
+    <t>thickness</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>Muro exterior</t>
+  </si>
+  <si>
+    <t>solar_absortivity</t>
+  </si>
+  <si>
+    <t>[0.8, 0.8]</t>
+  </si>
+  <si>
+    <t>materials</t>
+  </si>
+  <si>
+    <t>[Mortero cemento, Ladrillo hueco]</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>0.11</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Base de Datos</t>
-  </si>
-  <si>
-    <t>zonaB4</t>
-  </si>
-  <si>
-    <t>file_name</t>
-  </si>
-  <si>
-    <t>meteo/zonaB4.met</t>
-  </si>
-  <si>
-    <t>Mortero cemento</t>
-  </si>
-  <si>
-    <t>Ladrillo hueco</t>
-  </si>
-  <si>
     <t>conductivity</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>density</t>
-  </si>
-  <si>
-    <t>specific_heat</t>
-  </si>
-  <si>
-    <t>thickness</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>Muro exterior</t>
-  </si>
-  <si>
-    <t>solar_absortivity</t>
-  </si>
-  <si>
-    <t>[0.8, 0.8]</t>
-  </si>
-  <si>
-    <t>materials</t>
-  </si>
-  <si>
-    <t>[Mortero cemento, Ladrillo hueco]</t>
-  </si>
-  <si>
-    <t>0.49</t>
-  </si>
-  <si>
-    <t>0.11</t>
   </si>
 </sst>
 </file>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9360BA7A-1976-0F4A-8D53-E3E18BA52395}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,18 +497,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -533,18 +533,18 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAF5587-67B0-0644-B1B6-3B1582202EC6}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,27 +571,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>2000</v>
@@ -600,15 +600,15 @@
         <v>1050</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>1200</v>
@@ -617,7 +617,7 @@
         <v>920</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -642,24 +642,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>